<commit_message>
IMPLEMENTAÇÃO COMPLETA, SEPARADA E ORGANIZADA DAS COMISSÕES POR RECEBIMENTO
</commit_message>
<xml_diff>
--- a/Conversões.xlsx
+++ b/Conversões.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Código Produto</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>CS-Test</t>
+  </si>
+  <si>
+    <t>PENDENTE</t>
   </si>
   <si>
     <t>FATURADO</t>
@@ -568,31 +571,31 @@
         <v>45915</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -609,37 +612,37 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2">
         <v>45915</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -656,40 +659,40 @@
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
         <v>45920</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>